<commit_message>
add new column about label encoding information
</commit_message>
<xml_diff>
--- a/input/About_data.xlsx
+++ b/input/About_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/takuto/Desktop/Elo_kaggle/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B010D8-7721-4845-8817-0F7DF8F109F4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACAE8AD-1E58-684F-8E2E-A1A8558E7748}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{2E7745DE-49C9-0647-A133-0399E404AA1E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="133">
   <si>
     <t>テーブル名</t>
   </si>
@@ -550,6 +550,18 @@
     <rPh sb="0" eb="2">
       <t>テンポ</t>
     </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>merchant_label_id</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>numeric</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>merchant_idにlabel_encoding</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1638,11 +1650,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA66356-3ADB-4543-9D45-2E66A647BD0B}">
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="93" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -2112,7 +2124,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="5">
-        <f t="shared" ref="J18:J30" si="2">I18/29112361</f>
+        <f t="shared" ref="J18:J31" si="2">I18/29112361</f>
         <v>0</v>
       </c>
     </row>
@@ -2277,61 +2289,49 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E25" s="1">
-        <v>14</v>
-      </c>
-      <c r="F25" s="1">
-        <v>-13</v>
-      </c>
-      <c r="G25" s="1">
-        <v>0</v>
-      </c>
-      <c r="H25" s="1">
-        <v>-4.49</v>
+        <v>326311</v>
       </c>
       <c r="I25" s="1">
-        <v>0</v>
+        <v>138481</v>
       </c>
       <c r="J25" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4.7567766832789689E-3</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="E26" s="1">
-        <v>215014</v>
+        <v>14</v>
       </c>
       <c r="F26" s="1">
-        <v>-0.75</v>
+        <v>-13</v>
       </c>
       <c r="G26" s="1">
-        <v>6010603.9699999997</v>
+        <v>0</v>
       </c>
       <c r="H26" s="1">
-        <v>0.04</v>
+        <v>-4.49</v>
       </c>
       <c r="I26" s="1">
         <v>0</v>
@@ -2343,25 +2343,28 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E27" s="1">
-        <v>16395300</v>
-      </c>
-      <c r="F27" s="3">
-        <v>42736.000092592592</v>
-      </c>
-      <c r="G27" s="3">
-        <v>43159.999895833331</v>
+        <v>215014</v>
+      </c>
+      <c r="F27" s="1">
+        <v>-0.75</v>
+      </c>
+      <c r="G27" s="1">
+        <v>6010603.9699999997</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.04</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
@@ -2373,94 +2376,91 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E28" s="1">
-        <v>5</v>
-      </c>
-      <c r="F28" s="1">
-        <v>1</v>
-      </c>
-      <c r="G28" s="1">
-        <v>5</v>
-      </c>
-      <c r="H28" s="1">
-        <v>2.19</v>
+        <v>16395300</v>
+      </c>
+      <c r="F28" s="3">
+        <v>42736.000092592592</v>
+      </c>
+      <c r="G28" s="3">
+        <v>43159.999895833331</v>
       </c>
       <c r="I28" s="1">
-        <v>2652864</v>
+        <v>0</v>
       </c>
       <c r="J28" s="5">
         <f t="shared" si="2"/>
-        <v>9.1125003568072002E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="E29" s="1">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F29" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G29" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H29" s="1">
-        <v>10.57</v>
+        <v>2.19</v>
       </c>
       <c r="I29" s="1">
-        <v>0</v>
+        <v>2652864</v>
       </c>
       <c r="J29" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.1125003568072002E-2</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E30" s="1">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F30" s="1">
         <v>-1</v>
       </c>
       <c r="G30" s="1">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="H30" s="1">
-        <v>26.85</v>
+        <v>10.57</v>
       </c>
       <c r="I30" s="1">
         <v>0</v>
@@ -2471,120 +2471,129 @@
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" s="1">
+        <v>41</v>
+      </c>
+      <c r="F31" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G31" s="1">
+        <v>41</v>
+      </c>
+      <c r="H31" s="1">
+        <v>26.85</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2" t="s">
+      <c r="D32" s="2"/>
+      <c r="E32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="J32" s="2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E32" s="1">
-        <v>1</v>
-      </c>
-      <c r="I32" s="1">
-        <v>0</v>
-      </c>
-      <c r="J32" s="5">
-        <f>I32/1963031</f>
-        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="E33" s="1">
-        <v>290001</v>
+        <v>1</v>
       </c>
       <c r="I33" s="1">
         <v>0</v>
       </c>
       <c r="J33" s="5">
-        <f t="shared" ref="J33:J45" si="3">I33/1963031</f>
+        <f>I33/1963031</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>106</v>
+        <v>38</v>
       </c>
       <c r="E34" s="1">
-        <v>308</v>
-      </c>
-      <c r="F34" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G34" s="1">
-        <v>347</v>
-      </c>
-      <c r="H34" s="1">
-        <v>134.38999999999999</v>
+        <v>290001</v>
       </c>
       <c r="I34" s="1">
         <v>0</v>
       </c>
       <c r="J34" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J34:J47" si="3">I34/1963031</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E35" s="1">
-        <v>2</v>
+        <v>308</v>
+      </c>
+      <c r="F35" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G35" s="1">
+        <v>347</v>
+      </c>
+      <c r="H35" s="1">
+        <v>134.38999999999999</v>
       </c>
       <c r="I35" s="1">
         <v>0</v>
@@ -2596,28 +2605,19 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="E36" s="1">
-        <v>15</v>
-      </c>
-      <c r="F36" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G36" s="1">
-        <v>999</v>
-      </c>
-      <c r="H36" s="1">
-        <v>0.68</v>
+        <v>2</v>
       </c>
       <c r="I36" s="1">
         <v>0</v>
@@ -2629,166 +2629,157 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="E37" s="1">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="F37" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G37" s="1">
+        <v>999</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0.68</v>
       </c>
       <c r="I37" s="1">
-        <v>55922</v>
+        <v>0</v>
       </c>
       <c r="J37" s="5">
         <f t="shared" si="3"/>
-        <v>2.8487578647509896E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>44</v>
+        <v>108</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="E38" s="1">
-        <v>314</v>
-      </c>
-      <c r="F38" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G38" s="1">
-        <v>891</v>
-      </c>
-      <c r="H38" s="1">
-        <v>430.97</v>
+        <v>3</v>
       </c>
       <c r="I38" s="1">
-        <v>0</v>
+        <v>55922</v>
       </c>
       <c r="J38" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.8487578647509896E-2</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E39" s="1">
-        <v>226129</v>
+        <v>314</v>
+      </c>
+      <c r="F39" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G39" s="1">
+        <v>891</v>
+      </c>
+      <c r="H39" s="1">
+        <v>430.97</v>
       </c>
       <c r="I39" s="1">
-        <v>26216</v>
+        <v>0</v>
       </c>
       <c r="J39" s="5">
         <f t="shared" si="3"/>
-        <v>1.3354857870303627E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>128</v>
+        <v>46</v>
       </c>
       <c r="E40" s="1">
-        <v>2</v>
-      </c>
-      <c r="F40" s="1">
-        <v>1</v>
-      </c>
-      <c r="G40" s="1">
-        <v>2</v>
-      </c>
-      <c r="H40" s="1">
-        <v>1.48</v>
+        <v>226129</v>
       </c>
       <c r="I40" s="1">
-        <v>0</v>
+        <v>26216</v>
       </c>
       <c r="J40" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.3354857870303627E-2</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>47</v>
+        <v>131</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="E41" s="1">
-        <v>75190</v>
-      </c>
-      <c r="F41" s="1">
-        <v>-0.75</v>
-      </c>
-      <c r="G41" s="1">
-        <v>263.16000000000003</v>
-      </c>
-      <c r="H41" s="1">
-        <v>-0.55000000000000004</v>
+        <v>226129</v>
       </c>
       <c r="I41" s="1">
-        <v>0</v>
+        <v>26216</v>
       </c>
       <c r="J41" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.3354857870303627E-2</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="E42" s="1">
-        <v>1667025</v>
-      </c>
-      <c r="F42" s="3">
-        <v>42795.142256944448</v>
-      </c>
-      <c r="G42" s="3">
-        <v>43220.999988425923</v>
+        <v>2</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1</v>
+      </c>
+      <c r="G42" s="1">
+        <v>2</v>
+      </c>
+      <c r="H42" s="1">
+        <v>1.48</v>
       </c>
       <c r="I42" s="1">
         <v>0</v>
@@ -2800,61 +2791,58 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E43" s="1">
-        <v>5</v>
+        <v>75190</v>
       </c>
       <c r="F43" s="1">
-        <v>1</v>
+        <v>-0.75</v>
       </c>
       <c r="G43" s="1">
-        <v>5</v>
+        <v>263.16000000000003</v>
       </c>
       <c r="H43" s="1">
-        <v>2.2000000000000002</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="I43" s="1">
-        <v>111745</v>
+        <v>0</v>
       </c>
       <c r="J43" s="5">
         <f t="shared" si="3"/>
-        <v>5.6924725080755217E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E44" s="1">
-        <v>25</v>
-      </c>
-      <c r="F44" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G44" s="1">
-        <v>24</v>
-      </c>
-      <c r="H44" s="1">
-        <v>10.88</v>
+        <v>1667025</v>
+      </c>
+      <c r="F44" s="3">
+        <v>42795.142256944448</v>
+      </c>
+      <c r="G44" s="3">
+        <v>43220.999988425923</v>
       </c>
       <c r="I44" s="1">
         <v>0</v>
@@ -2866,230 +2854,227 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="E45" s="1">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="F45" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G45" s="1">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="H45" s="1">
-        <v>25.98</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I45" s="1">
-        <v>0</v>
+        <v>111745</v>
       </c>
       <c r="J45" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6924725080755217E-2</v>
       </c>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>12</v>
+      <c r="A46" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E46" s="1">
+        <v>25</v>
+      </c>
+      <c r="F46" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G46" s="1">
+        <v>24</v>
+      </c>
+      <c r="H46" s="1">
+        <v>10.88</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0</v>
+      </c>
+      <c r="J46" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>129</v>
+        <v>45</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="E47" s="1">
-        <v>334633</v>
+        <v>41</v>
+      </c>
+      <c r="F47" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G47" s="1">
+        <v>41</v>
+      </c>
+      <c r="H47" s="1">
+        <v>25.98</v>
       </c>
       <c r="I47" s="1">
         <v>0</v>
       </c>
       <c r="J47" s="5">
-        <f>I47/334696</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E48" s="1">
-        <v>109391</v>
-      </c>
-      <c r="F48" s="1">
-        <v>1</v>
-      </c>
-      <c r="G48" s="1">
-        <v>112586</v>
-      </c>
-      <c r="H48" s="1">
-        <v>31028.74</v>
-      </c>
-      <c r="I48" s="1">
-        <v>0</v>
-      </c>
-      <c r="J48" s="5">
-        <f t="shared" ref="J48:J68" si="4">I48/334696</f>
-        <v>0</v>
+      <c r="A48" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="E49" s="1">
-        <v>324</v>
-      </c>
-      <c r="F49" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G49" s="1">
-        <v>891</v>
-      </c>
-      <c r="H49" s="1">
-        <v>423.13</v>
+        <v>334633</v>
       </c>
       <c r="I49" s="1">
         <v>0</v>
       </c>
       <c r="J49" s="5">
-        <f t="shared" si="4"/>
+        <f>I49/334696</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>70</v>
+        <v>131</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="E50" s="1">
-        <v>41</v>
-      </c>
-      <c r="F50" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G50" s="1">
-        <v>41</v>
-      </c>
-      <c r="H50" s="1">
-        <v>25.12</v>
+        <v>334633</v>
       </c>
       <c r="I50" s="1">
         <v>0</v>
       </c>
       <c r="J50" s="5">
-        <f t="shared" si="4"/>
+        <f>I50/334696</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>125</v>
+        <v>68</v>
       </c>
       <c r="E51" s="1">
-        <v>954</v>
+        <v>109391</v>
       </c>
       <c r="F51" s="1">
-        <v>-0.06</v>
+        <v>1</v>
       </c>
       <c r="G51" s="1">
-        <v>183.74</v>
+        <v>112586</v>
       </c>
       <c r="H51" s="1">
-        <v>0.01</v>
+        <v>31028.74</v>
       </c>
       <c r="I51" s="1">
         <v>0</v>
       </c>
       <c r="J51" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="J51:J71" si="4">I51/334696</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="1" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E52" s="1">
-        <v>947</v>
+        <v>324</v>
       </c>
       <c r="F52" s="1">
-        <v>-0.06</v>
+        <v>-1</v>
       </c>
       <c r="G52" s="1">
-        <v>182.08</v>
+        <v>891</v>
       </c>
       <c r="H52" s="1">
-        <v>0.01</v>
+        <v>423.13</v>
       </c>
       <c r="I52" s="1">
         <v>0</v>
@@ -3101,16 +3086,25 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="E53" s="1">
-        <v>2</v>
+        <v>41</v>
+      </c>
+      <c r="F53" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G53" s="1">
+        <v>41</v>
+      </c>
+      <c r="H53" s="1">
+        <v>25.12</v>
       </c>
       <c r="I53" s="1">
         <v>0</v>
@@ -3122,16 +3116,25 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E54" s="1">
-        <v>5</v>
+        <v>954</v>
+      </c>
+      <c r="F54" s="1">
+        <v>-0.06</v>
+      </c>
+      <c r="G54" s="1">
+        <v>183.74</v>
+      </c>
+      <c r="H54" s="1">
+        <v>0.01</v>
       </c>
       <c r="I54" s="1">
         <v>0</v>
@@ -3143,16 +3146,25 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E55" s="1">
-        <v>5</v>
+        <v>947</v>
+      </c>
+      <c r="F55" s="1">
+        <v>-0.06</v>
+      </c>
+      <c r="G55" s="1">
+        <v>182.08</v>
+      </c>
+      <c r="H55" s="1">
+        <v>0.01</v>
       </c>
       <c r="I55" s="1">
         <v>0</v>
@@ -3164,94 +3176,58 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="1" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="E56" s="1">
-        <v>3372</v>
-      </c>
-      <c r="F56" s="1">
-        <v>-82.13</v>
-      </c>
-      <c r="G56" s="1">
-        <v>851844.64</v>
-      </c>
-      <c r="H56" s="1">
-        <v>13.83</v>
+        <v>2</v>
       </c>
       <c r="I56" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="J56" s="5">
         <f t="shared" si="4"/>
-        <v>3.8841217104476896E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="E57" s="1">
-        <v>100002</v>
-      </c>
-      <c r="F57" s="1">
-        <v>0.33</v>
-      </c>
-      <c r="G57" s="1">
-        <v>61851.33</v>
-      </c>
-      <c r="H57" s="1">
-        <v>1.59</v>
+        <v>5</v>
       </c>
       <c r="I57" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J57" s="5">
         <f t="shared" si="4"/>
-        <v>8.9633577933408233E-6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="E58" s="1">
-        <v>3</v>
-      </c>
-      <c r="F58" s="1">
-        <v>1</v>
-      </c>
-      <c r="G58" s="1">
-        <v>3</v>
-      </c>
-      <c r="H58" s="1">
-        <v>2.99</v>
+        <v>5</v>
       </c>
       <c r="I58" s="1">
         <v>0</v>
@@ -3263,28 +3239,28 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E59" s="1">
-        <v>4507</v>
+        <v>3372</v>
       </c>
       <c r="F59" s="1">
         <v>-82.13</v>
       </c>
       <c r="G59" s="1">
-        <v>1513959</v>
+        <v>851844.64</v>
       </c>
       <c r="H59" s="1">
-        <v>21.65</v>
+        <v>13.83</v>
       </c>
       <c r="I59" s="1">
         <v>13</v>
@@ -3296,28 +3272,28 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E60" s="1">
-        <v>135201</v>
+        <v>100002</v>
       </c>
       <c r="F60" s="1">
-        <v>0.17</v>
+        <v>0.33</v>
       </c>
       <c r="G60" s="1">
-        <v>56077.5</v>
+        <v>61851.33</v>
       </c>
       <c r="H60" s="1">
-        <v>1.89</v>
+        <v>1.59</v>
       </c>
       <c r="I60" s="1">
         <v>3</v>
@@ -3329,28 +3305,28 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E61" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F61" s="1">
         <v>1</v>
       </c>
       <c r="G61" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H61" s="1">
-        <v>5.95</v>
+        <v>2.99</v>
       </c>
       <c r="I61" s="1">
         <v>0</v>
@@ -3362,28 +3338,28 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E62" s="1">
-        <v>5009</v>
+        <v>4507</v>
       </c>
       <c r="F62" s="1">
         <v>-82.13</v>
       </c>
       <c r="G62" s="1">
-        <v>2567408</v>
+        <v>1513959</v>
       </c>
       <c r="H62" s="1">
-        <v>25.23</v>
+        <v>21.65</v>
       </c>
       <c r="I62" s="1">
         <v>13</v>
@@ -3395,28 +3371,28 @@
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E63" s="1">
-        <v>172916</v>
+        <v>135201</v>
       </c>
       <c r="F63" s="1">
-        <v>0.1</v>
+        <v>0.17</v>
       </c>
       <c r="G63" s="1">
-        <v>50215.56</v>
+        <v>56077.5</v>
       </c>
       <c r="H63" s="1">
-        <v>2.08</v>
+        <v>1.89</v>
       </c>
       <c r="I63" s="1">
         <v>3</v>
@@ -3428,28 +3404,28 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E64" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F64" s="1">
         <v>1</v>
       </c>
       <c r="G64" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H64" s="1">
-        <v>11.6</v>
+        <v>5.95</v>
       </c>
       <c r="I64" s="1">
         <v>0</v>
@@ -3461,76 +3437,94 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>117</v>
+        <v>80</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="E65" s="1">
-        <v>2</v>
+        <v>5009</v>
+      </c>
+      <c r="F65" s="1">
+        <v>-82.13</v>
+      </c>
+      <c r="G65" s="1">
+        <v>2567408</v>
+      </c>
+      <c r="H65" s="1">
+        <v>25.23</v>
       </c>
       <c r="I65" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J65" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.8841217104476896E-5</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="1" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>48</v>
+        <v>81</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="E66" s="1">
-        <v>271</v>
+        <v>172916</v>
       </c>
       <c r="F66" s="1">
-        <v>-1</v>
+        <v>0.1</v>
       </c>
       <c r="G66" s="1">
-        <v>347</v>
+        <v>50215.56</v>
       </c>
       <c r="H66" s="1">
-        <v>102.92</v>
+        <v>2.08</v>
       </c>
       <c r="I66" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J66" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8.9633577933408233E-6</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="1" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>49</v>
+        <v>82</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="E67" s="1">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F67" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G67" s="1">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="H67" s="1">
-        <v>11.86</v>
+        <v>11.6</v>
       </c>
       <c r="I67" s="1">
         <v>0</v>
@@ -3542,30 +3536,111 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E68" s="1">
+        <v>2</v>
+      </c>
+      <c r="I68" s="1">
+        <v>0</v>
+      </c>
+      <c r="J68" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E69" s="1">
+        <v>271</v>
+      </c>
+      <c r="F69" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G69" s="1">
+        <v>347</v>
+      </c>
+      <c r="H69" s="1">
+        <v>102.92</v>
+      </c>
+      <c r="I69" s="1">
+        <v>0</v>
+      </c>
+      <c r="J69" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E70" s="1">
+        <v>25</v>
+      </c>
+      <c r="F70" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G70" s="1">
+        <v>24</v>
+      </c>
+      <c r="H70" s="1">
+        <v>11.86</v>
+      </c>
+      <c r="I70" s="1">
+        <v>0</v>
+      </c>
+      <c r="J70" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E71" s="1">
         <v>5</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F71" s="1">
         <v>1</v>
       </c>
-      <c r="G68" s="1">
+      <c r="G71" s="1">
         <v>5</v>
       </c>
-      <c r="H68" s="1">
+      <c r="H71" s="1">
         <v>2.38</v>
       </c>
-      <c r="I68" s="1">
+      <c r="I71" s="1">
         <v>11887</v>
       </c>
-      <c r="J68" s="5">
+      <c r="J71" s="5">
         <f t="shared" si="4"/>
         <v>3.5515811363147451E-2</v>
       </c>

</xml_diff>

<commit_message>
add target class and mark feature columns
</commit_message>
<xml_diff>
--- a/input/About_data.xlsx
+++ b/input/About_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/takuto/Desktop/Elo_kaggle/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8713277D-C17A-7444-9902-5AA062FFED57}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76844748-B5E6-724C-B57E-FAF26FA9D6EE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{2E7745DE-49C9-0647-A133-0399E404AA1E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="140">
   <si>
     <t>テーブル名</t>
   </si>
@@ -576,6 +576,25 @@
     <t>train data, test dataで一致はない</t>
     <phoneticPr fontId="2"/>
   </si>
+  <si>
+    <t>target_class</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>targetにおいて, -30&lt;:1, -30&gt;=かつ 0&lt;:2 , 0&gt;=: 3とする</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(1:2207, 2:100471, 3:99239)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>物理名 (青字は非特徴量)</t>
+    <rPh sb="0" eb="2">
+      <t>アオジ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
 </sst>
 </file>
 
@@ -584,7 +603,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -610,6 +629,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF0070C0"/>
+      <name val="メイリオ"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
       <name val="メイリオ"/>
       <family val="2"/>
       <charset val="128"/>
@@ -649,7 +675,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -669,6 +695,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1662,11 +1691,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA66356-3ADB-4543-9D45-2E66A647BD0B}">
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="86" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C30" sqref="C30"/>
+      <selection pane="topRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1690,7 +1719,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>139</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -1737,7 +1766,7 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1764,7 +1793,7 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1783,7 +1812,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="5">
-        <f t="shared" ref="J5:J9" si="0">I5/201917</f>
+        <f t="shared" ref="J5:J10" si="0">I5/201917</f>
         <v>0</v>
       </c>
     </row>
@@ -1878,26 +1907,26 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
+      <c r="A9" s="7" t="s">
+        <v>136</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>138</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="E9" s="1">
-        <v>197110</v>
+        <v>3</v>
       </c>
       <c r="F9" s="1">
-        <v>-33.22</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1">
-        <v>17.97</v>
-      </c>
-      <c r="H9" s="1">
-        <v>-0.39</v>
+        <v>3</v>
       </c>
       <c r="I9" s="1">
         <v>0</v>
@@ -1908,117 +1937,117 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1">
+        <v>197110</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-33.22</v>
+      </c>
+      <c r="G10" s="1">
+        <v>17.97</v>
+      </c>
+      <c r="H10" s="1">
+        <v>-0.39</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:10">
+      <c r="A12" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="1">
-        <v>75</v>
-      </c>
-      <c r="F11" s="4">
-        <v>40848</v>
-      </c>
-      <c r="G11" s="4">
-        <v>43101</v>
-      </c>
-      <c r="I11" s="1">
-        <v>1</v>
-      </c>
-      <c r="J11" s="5">
-        <f>I11/123623</f>
-        <v>8.0891096317028384E-6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1">
+        <v>75</v>
+      </c>
+      <c r="F12" s="4">
+        <v>40848</v>
+      </c>
+      <c r="G12" s="4">
+        <v>43101</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5">
+        <f>I12/123623</f>
+        <v>8.0891096317028384E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E13" s="1">
         <v>123623</v>
       </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5">
-        <f t="shared" ref="J12:J14" si="1">I12/123623</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="1">
-        <v>5</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1">
-        <v>5</v>
-      </c>
-      <c r="H13" s="1">
-        <v>3.11</v>
-      </c>
       <c r="I13" s="1">
         <v>0</v>
       </c>
       <c r="J13" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J13:J15" si="1">I13/123623</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>86</v>
@@ -2027,16 +2056,16 @@
         <v>21</v>
       </c>
       <c r="E14" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
       </c>
       <c r="G14" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H14" s="1">
-        <v>1.74</v>
+        <v>3.11</v>
       </c>
       <c r="I14" s="1">
         <v>0</v>
@@ -2048,7 +2077,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>86</v>
@@ -2057,140 +2086,146 @@
         <v>21</v>
       </c>
       <c r="E15" s="1">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <v>3</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1.74</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1">
         <v>2</v>
       </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
         <v>1</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H16" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15" s="5">
-        <f>I15/123623</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="2" t="s">
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <f>I16/123623</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="1">
-        <v>2</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0</v>
-      </c>
-      <c r="J17" s="5">
-        <f>I17/29112361</f>
-        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="E18" s="1">
-        <v>325540</v>
+        <v>2</v>
       </c>
       <c r="I18" s="1">
         <v>0</v>
       </c>
       <c r="J18" s="5">
-        <f t="shared" ref="J18:J31" si="2">I18/29112361</f>
+        <f>I18/29112361</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="E19" s="1">
-        <v>308</v>
-      </c>
-      <c r="F19" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G19" s="1">
-        <v>347</v>
+        <v>325540</v>
       </c>
       <c r="I19" s="1">
         <v>0</v>
       </c>
       <c r="J19" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J19:J32" si="2">I19/29112361</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>109</v>
+        <v>48</v>
       </c>
       <c r="E20" s="1">
-        <v>2</v>
+        <v>308</v>
+      </c>
+      <c r="F20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>347</v>
       </c>
       <c r="I20" s="1">
         <v>0</v>
@@ -2202,28 +2237,19 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="E21" s="1">
-        <v>15</v>
-      </c>
-      <c r="F21" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G21" s="1">
-        <v>999</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0.65</v>
+        <v>2</v>
       </c>
       <c r="I21" s="1">
         <v>0</v>
@@ -2235,88 +2261,100 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="E22" s="1">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="F22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>999</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.65</v>
       </c>
       <c r="I22" s="1">
-        <v>178159</v>
+        <v>0</v>
       </c>
       <c r="J22" s="5">
         <f t="shared" si="2"/>
-        <v>6.1197028987102766E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>44</v>
+        <v>98</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="E23" s="1">
-        <v>327</v>
-      </c>
-      <c r="F23" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G23" s="1">
-        <v>891</v>
-      </c>
-      <c r="H23" s="1">
-        <v>481.01</v>
+        <v>3</v>
       </c>
       <c r="I23" s="1">
-        <v>0</v>
+        <v>178159</v>
       </c>
       <c r="J23" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.1197028987102766E-3</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E24" s="1">
-        <v>326311</v>
+        <v>327</v>
+      </c>
+      <c r="F24" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>891</v>
+      </c>
+      <c r="H24" s="1">
+        <v>481.01</v>
       </c>
       <c r="I24" s="1">
-        <v>138481</v>
+        <v>0</v>
       </c>
       <c r="J24" s="5">
         <f t="shared" si="2"/>
-        <v>4.7567766832789689E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="1" t="s">
-        <v>130</v>
+      <c r="A25" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>132</v>
+        <v>91</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="E25" s="1">
         <v>326311</v>
@@ -2331,61 +2369,49 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E26" s="1">
-        <v>14</v>
-      </c>
-      <c r="F26" s="1">
-        <v>-13</v>
-      </c>
-      <c r="G26" s="1">
-        <v>0</v>
-      </c>
-      <c r="H26" s="1">
-        <v>-4.49</v>
+        <v>326311</v>
       </c>
       <c r="I26" s="1">
-        <v>0</v>
+        <v>138481</v>
       </c>
       <c r="J26" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4.7567766832789689E-3</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="E27" s="1">
-        <v>215014</v>
+        <v>14</v>
       </c>
       <c r="F27" s="1">
-        <v>-0.75</v>
+        <v>-13</v>
       </c>
       <c r="G27" s="1">
-        <v>6010603.9699999997</v>
+        <v>0</v>
       </c>
       <c r="H27" s="1">
-        <v>0.04</v>
+        <v>-4.49</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
@@ -2397,25 +2423,28 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E28" s="1">
-        <v>16395300</v>
-      </c>
-      <c r="F28" s="3">
-        <v>42736.000092592592</v>
-      </c>
-      <c r="G28" s="3">
-        <v>43159.999895833331</v>
+        <v>215014</v>
+      </c>
+      <c r="F28" s="1">
+        <v>-0.75</v>
+      </c>
+      <c r="G28" s="1">
+        <v>6010603.9699999997</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0.04</v>
       </c>
       <c r="I28" s="1">
         <v>0</v>
@@ -2426,95 +2455,92 @@
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="1" t="s">
-        <v>37</v>
+      <c r="A29" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E29" s="1">
-        <v>5</v>
-      </c>
-      <c r="F29" s="1">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1">
-        <v>5</v>
-      </c>
-      <c r="H29" s="1">
-        <v>2.19</v>
+        <v>16395300</v>
+      </c>
+      <c r="F29" s="3">
+        <v>42736.000092592592</v>
+      </c>
+      <c r="G29" s="3">
+        <v>43159.999895833331</v>
       </c>
       <c r="I29" s="1">
-        <v>2652864</v>
+        <v>0</v>
       </c>
       <c r="J29" s="5">
         <f t="shared" si="2"/>
-        <v>9.1125003568072002E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="E30" s="1">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F30" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G30" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H30" s="1">
-        <v>10.57</v>
+        <v>2.19</v>
       </c>
       <c r="I30" s="1">
-        <v>0</v>
+        <v>2652864</v>
       </c>
       <c r="J30" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.1125003568072002E-2</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E31" s="1">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F31" s="1">
         <v>-1</v>
       </c>
       <c r="G31" s="1">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="H31" s="1">
-        <v>26.85</v>
+        <v>10.57</v>
       </c>
       <c r="I31" s="1">
         <v>0</v>
@@ -2525,123 +2551,132 @@
       </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="1">
+        <v>41</v>
+      </c>
+      <c r="F32" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G32" s="1">
+        <v>41</v>
+      </c>
+      <c r="H32" s="1">
+        <v>26.85</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
+      <c r="J32" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2" t="s">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2" t="s">
+      <c r="D33" s="2"/>
+      <c r="E33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="J33" s="2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E33" s="1">
-        <v>1</v>
-      </c>
-      <c r="I33" s="1">
-        <v>0</v>
-      </c>
-      <c r="J33" s="5">
-        <f>I33/1963031</f>
-        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="E34" s="1">
-        <v>290001</v>
+        <v>1</v>
       </c>
       <c r="I34" s="1">
         <v>0</v>
       </c>
       <c r="J34" s="5">
-        <f t="shared" ref="J34:J47" si="3">I34/1963031</f>
+        <f>I34/1963031</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>106</v>
+        <v>38</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="E35" s="1">
-        <v>308</v>
-      </c>
-      <c r="F35" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G35" s="1">
-        <v>347</v>
-      </c>
-      <c r="H35" s="1">
-        <v>134.38999999999999</v>
+        <v>290001</v>
       </c>
       <c r="I35" s="1">
         <v>0</v>
       </c>
       <c r="J35" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J35:J48" si="3">I35/1963031</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E36" s="1">
-        <v>2</v>
+        <v>308</v>
+      </c>
+      <c r="F36" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G36" s="1">
+        <v>347</v>
+      </c>
+      <c r="H36" s="1">
+        <v>134.38999999999999</v>
       </c>
       <c r="I36" s="1">
         <v>0</v>
@@ -2653,28 +2688,19 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="E37" s="1">
-        <v>15</v>
-      </c>
-      <c r="F37" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G37" s="1">
-        <v>999</v>
-      </c>
-      <c r="H37" s="1">
-        <v>0.68</v>
+        <v>2</v>
       </c>
       <c r="I37" s="1">
         <v>0</v>
@@ -2686,88 +2712,100 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="E38" s="1">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="F38" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G38" s="1">
+        <v>999</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0.68</v>
       </c>
       <c r="I38" s="1">
-        <v>55922</v>
+        <v>0</v>
       </c>
       <c r="J38" s="5">
         <f t="shared" si="3"/>
-        <v>2.8487578647509896E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>44</v>
+        <v>108</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="E39" s="1">
-        <v>314</v>
-      </c>
-      <c r="F39" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G39" s="1">
-        <v>891</v>
-      </c>
-      <c r="H39" s="1">
-        <v>430.97</v>
+        <v>3</v>
       </c>
       <c r="I39" s="1">
-        <v>0</v>
+        <v>55922</v>
       </c>
       <c r="J39" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.8487578647509896E-2</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E40" s="1">
-        <v>226129</v>
+        <v>314</v>
+      </c>
+      <c r="F40" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G40" s="1">
+        <v>891</v>
+      </c>
+      <c r="H40" s="1">
+        <v>430.97</v>
       </c>
       <c r="I40" s="1">
-        <v>26216</v>
+        <v>0</v>
       </c>
       <c r="J40" s="5">
         <f t="shared" si="3"/>
-        <v>1.3354857870303627E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="1" t="s">
-        <v>130</v>
+      <c r="A41" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>132</v>
+        <v>91</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="E41" s="1">
         <v>226129</v>
@@ -2782,61 +2820,49 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="1" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E42" s="1">
-        <v>2</v>
-      </c>
-      <c r="F42" s="1">
-        <v>1</v>
-      </c>
-      <c r="G42" s="1">
-        <v>2</v>
-      </c>
-      <c r="H42" s="1">
-        <v>1.48</v>
+        <v>226129</v>
       </c>
       <c r="I42" s="1">
-        <v>0</v>
+        <v>26216</v>
       </c>
       <c r="J42" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.3354857870303627E-2</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="E43" s="1">
-        <v>75190</v>
+        <v>2</v>
       </c>
       <c r="F43" s="1">
-        <v>-0.75</v>
+        <v>1</v>
       </c>
       <c r="G43" s="1">
-        <v>263.16000000000003</v>
+        <v>2</v>
       </c>
       <c r="H43" s="1">
-        <v>-0.55000000000000004</v>
+        <v>1.48</v>
       </c>
       <c r="I43" s="1">
         <v>0</v>
@@ -2848,25 +2874,28 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E44" s="1">
-        <v>1667025</v>
-      </c>
-      <c r="F44" s="3">
-        <v>42795.142256944448</v>
-      </c>
-      <c r="G44" s="3">
-        <v>43220.999988425923</v>
+        <v>75190</v>
+      </c>
+      <c r="F44" s="1">
+        <v>-0.75</v>
+      </c>
+      <c r="G44" s="1">
+        <v>263.16000000000003</v>
+      </c>
+      <c r="H44" s="1">
+        <v>-0.55000000000000004</v>
       </c>
       <c r="I44" s="1">
         <v>0</v>
@@ -2877,95 +2906,92 @@
       </c>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="1" t="s">
-        <v>37</v>
+      <c r="A45" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E45" s="1">
-        <v>5</v>
-      </c>
-      <c r="F45" s="1">
-        <v>1</v>
-      </c>
-      <c r="G45" s="1">
-        <v>5</v>
-      </c>
-      <c r="H45" s="1">
-        <v>2.2000000000000002</v>
+        <v>1667025</v>
+      </c>
+      <c r="F45" s="3">
+        <v>42795.142256944448</v>
+      </c>
+      <c r="G45" s="3">
+        <v>43220.999988425923</v>
       </c>
       <c r="I45" s="1">
-        <v>111745</v>
+        <v>0</v>
       </c>
       <c r="J45" s="5">
         <f t="shared" si="3"/>
-        <v>5.6924725080755217E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="E46" s="1">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F46" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G46" s="1">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="H46" s="1">
-        <v>10.88</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I46" s="1">
-        <v>0</v>
+        <v>111745</v>
       </c>
       <c r="J46" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6924725080755217E-2</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E47" s="1">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F47" s="1">
         <v>-1</v>
       </c>
       <c r="G47" s="1">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="H47" s="1">
-        <v>25.98</v>
+        <v>10.88</v>
       </c>
       <c r="I47" s="1">
         <v>0</v>
@@ -2976,66 +3002,78 @@
       </c>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E48" s="1">
+        <v>41</v>
+      </c>
+      <c r="F48" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G48" s="1">
+        <v>41</v>
+      </c>
+      <c r="H48" s="1">
+        <v>25.98</v>
+      </c>
+      <c r="I48" s="1">
+        <v>0</v>
+      </c>
+      <c r="J48" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2" t="s">
+      <c r="B49" s="2"/>
+      <c r="C49" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2" t="s">
+      <c r="D49" s="2"/>
+      <c r="E49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="I49" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="J49" s="2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
-      <c r="A49" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E49" s="1">
-        <v>334633</v>
-      </c>
-      <c r="I49" s="1">
-        <v>0</v>
-      </c>
-      <c r="J49" s="5">
-        <f>I49/334696</f>
-        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
-        <v>130</v>
+        <v>33</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>132</v>
+        <v>91</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="E50" s="1">
         <v>334633</v>
@@ -3050,85 +3088,76 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="1" t="s">
-        <v>52</v>
+        <v>130</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="E51" s="1">
-        <v>109391</v>
-      </c>
-      <c r="F51" s="1">
-        <v>1</v>
-      </c>
-      <c r="G51" s="1">
-        <v>112586</v>
-      </c>
-      <c r="H51" s="1">
-        <v>31028.74</v>
+        <v>334633</v>
       </c>
       <c r="I51" s="1">
         <v>0</v>
       </c>
       <c r="J51" s="5">
-        <f t="shared" ref="J51:J71" si="4">I51/334696</f>
+        <f>I51/334696</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E52" s="1">
-        <v>324</v>
+        <v>109391</v>
       </c>
       <c r="F52" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G52" s="1">
-        <v>891</v>
+        <v>112586</v>
       </c>
       <c r="H52" s="1">
-        <v>423.13</v>
+        <v>31028.74</v>
       </c>
       <c r="I52" s="1">
         <v>0</v>
       </c>
       <c r="J52" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="J52:J72" si="4">I52/334696</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E53" s="1">
-        <v>41</v>
+        <v>324</v>
       </c>
       <c r="F53" s="1">
         <v>-1</v>
       </c>
       <c r="G53" s="1">
-        <v>41</v>
+        <v>891</v>
       </c>
       <c r="H53" s="1">
-        <v>25.12</v>
+        <v>423.13</v>
       </c>
       <c r="I53" s="1">
         <v>0</v>
@@ -3140,25 +3169,25 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>125</v>
+        <v>70</v>
       </c>
       <c r="E54" s="1">
-        <v>954</v>
+        <v>41</v>
       </c>
       <c r="F54" s="1">
-        <v>-0.06</v>
+        <v>-1</v>
       </c>
       <c r="G54" s="1">
-        <v>183.74</v>
+        <v>41</v>
       </c>
       <c r="H54" s="1">
-        <v>0.01</v>
+        <v>25.12</v>
       </c>
       <c r="I54" s="1">
         <v>0</v>
@@ -3170,22 +3199,22 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>71</v>
+        <v>125</v>
       </c>
       <c r="E55" s="1">
-        <v>947</v>
+        <v>954</v>
       </c>
       <c r="F55" s="1">
         <v>-0.06</v>
       </c>
       <c r="G55" s="1">
-        <v>182.08</v>
+        <v>183.74</v>
       </c>
       <c r="H55" s="1">
         <v>0.01</v>
@@ -3200,16 +3229,25 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="1" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="E56" s="1">
-        <v>2</v>
+        <v>947</v>
+      </c>
+      <c r="F56" s="1">
+        <v>-0.06</v>
+      </c>
+      <c r="G56" s="1">
+        <v>182.08</v>
+      </c>
+      <c r="H56" s="1">
+        <v>0.01</v>
       </c>
       <c r="I56" s="1">
         <v>0</v>
@@ -3221,16 +3259,16 @@
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="1" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="E57" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I57" s="1">
         <v>0</v>
@@ -3242,13 +3280,13 @@
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="E58" s="1">
         <v>5</v>
@@ -3263,313 +3301,313 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>115</v>
+        <v>73</v>
       </c>
       <c r="E59" s="1">
-        <v>3372</v>
-      </c>
-      <c r="F59" s="1">
-        <v>-82.13</v>
-      </c>
-      <c r="G59" s="1">
-        <v>851844.64</v>
-      </c>
-      <c r="H59" s="1">
-        <v>13.83</v>
+        <v>5</v>
       </c>
       <c r="I59" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="J59" s="5">
         <f t="shared" si="4"/>
-        <v>3.8841217104476896E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E60" s="1">
-        <v>100002</v>
+        <v>3372</v>
       </c>
       <c r="F60" s="1">
-        <v>0.33</v>
+        <v>-82.13</v>
       </c>
       <c r="G60" s="1">
-        <v>61851.33</v>
+        <v>851844.64</v>
       </c>
       <c r="H60" s="1">
-        <v>1.59</v>
+        <v>13.83</v>
       </c>
       <c r="I60" s="1">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="J60" s="5">
         <f t="shared" si="4"/>
-        <v>8.9633577933408233E-6</v>
+        <v>3.8841217104476896E-5</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E61" s="1">
+        <v>100002</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="G61" s="1">
+        <v>61851.33</v>
+      </c>
+      <c r="H61" s="1">
+        <v>1.59</v>
+      </c>
+      <c r="I61" s="1">
         <v>3</v>
-      </c>
-      <c r="F61" s="1">
-        <v>1</v>
-      </c>
-      <c r="G61" s="1">
-        <v>3</v>
-      </c>
-      <c r="H61" s="1">
-        <v>2.99</v>
-      </c>
-      <c r="I61" s="1">
-        <v>0</v>
       </c>
       <c r="J61" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8.9633577933408233E-6</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E62" s="1">
-        <v>4507</v>
+        <v>3</v>
       </c>
       <c r="F62" s="1">
-        <v>-82.13</v>
+        <v>1</v>
       </c>
       <c r="G62" s="1">
-        <v>1513959</v>
+        <v>3</v>
       </c>
       <c r="H62" s="1">
-        <v>21.65</v>
+        <v>2.99</v>
       </c>
       <c r="I62" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="J62" s="5">
         <f t="shared" si="4"/>
-        <v>3.8841217104476896E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E63" s="1">
-        <v>135201</v>
+        <v>4507</v>
       </c>
       <c r="F63" s="1">
-        <v>0.17</v>
+        <v>-82.13</v>
       </c>
       <c r="G63" s="1">
-        <v>56077.5</v>
+        <v>1513959</v>
       </c>
       <c r="H63" s="1">
-        <v>1.89</v>
+        <v>21.65</v>
       </c>
       <c r="I63" s="1">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="J63" s="5">
         <f t="shared" si="4"/>
-        <v>8.9633577933408233E-6</v>
+        <v>3.8841217104476896E-5</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E64" s="1">
-        <v>6</v>
+        <v>135201</v>
       </c>
       <c r="F64" s="1">
-        <v>1</v>
+        <v>0.17</v>
       </c>
       <c r="G64" s="1">
-        <v>6</v>
+        <v>56077.5</v>
       </c>
       <c r="H64" s="1">
-        <v>5.95</v>
+        <v>1.89</v>
       </c>
       <c r="I64" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J64" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8.9633577933408233E-6</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E65" s="1">
-        <v>5009</v>
+        <v>6</v>
       </c>
       <c r="F65" s="1">
-        <v>-82.13</v>
+        <v>1</v>
       </c>
       <c r="G65" s="1">
-        <v>2567408</v>
+        <v>6</v>
       </c>
       <c r="H65" s="1">
-        <v>25.23</v>
+        <v>5.95</v>
       </c>
       <c r="I65" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="J65" s="5">
         <f t="shared" si="4"/>
-        <v>3.8841217104476896E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E66" s="1">
-        <v>172916</v>
+        <v>5009</v>
       </c>
       <c r="F66" s="1">
-        <v>0.1</v>
+        <v>-82.13</v>
       </c>
       <c r="G66" s="1">
-        <v>50215.56</v>
+        <v>2567408</v>
       </c>
       <c r="H66" s="1">
-        <v>2.08</v>
+        <v>25.23</v>
       </c>
       <c r="I66" s="1">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="J66" s="5">
         <f t="shared" si="4"/>
-        <v>8.9633577933408233E-6</v>
+        <v>3.8841217104476896E-5</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E67" s="1">
-        <v>12</v>
+        <v>172916</v>
       </c>
       <c r="F67" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="G67" s="1">
-        <v>12</v>
+        <v>50215.56</v>
       </c>
       <c r="H67" s="1">
-        <v>11.6</v>
+        <v>2.08</v>
       </c>
       <c r="I67" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J67" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8.9633577933408233E-6</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>117</v>
+        <v>82</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="E68" s="1">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="F68" s="1">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1">
+        <v>12</v>
+      </c>
+      <c r="H68" s="1">
+        <v>11.6</v>
       </c>
       <c r="I68" s="1">
         <v>0</v>
@@ -3581,25 +3619,16 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="1" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>48</v>
+        <v>117</v>
       </c>
       <c r="E69" s="1">
-        <v>271</v>
-      </c>
-      <c r="F69" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G69" s="1">
-        <v>347</v>
-      </c>
-      <c r="H69" s="1">
-        <v>102.92</v>
+        <v>2</v>
       </c>
       <c r="I69" s="1">
         <v>0</v>
@@ -3611,25 +3640,25 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E70" s="1">
-        <v>25</v>
+        <v>271</v>
       </c>
       <c r="F70" s="1">
         <v>-1</v>
       </c>
       <c r="G70" s="1">
-        <v>24</v>
+        <v>347</v>
       </c>
       <c r="H70" s="1">
-        <v>11.86</v>
+        <v>102.92</v>
       </c>
       <c r="I70" s="1">
         <v>0</v>
@@ -3641,30 +3670,60 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E71" s="1">
+        <v>25</v>
+      </c>
+      <c r="F71" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G71" s="1">
+        <v>24</v>
+      </c>
+      <c r="H71" s="1">
+        <v>11.86</v>
+      </c>
+      <c r="I71" s="1">
+        <v>0</v>
+      </c>
+      <c r="J71" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E72" s="1">
         <v>5</v>
       </c>
-      <c r="F71" s="1">
+      <c r="F72" s="1">
         <v>1</v>
       </c>
-      <c r="G71" s="1">
+      <c r="G72" s="1">
         <v>5</v>
       </c>
-      <c r="H71" s="1">
+      <c r="H72" s="1">
         <v>2.38</v>
       </c>
-      <c r="I71" s="1">
+      <c r="I72" s="1">
         <v>11887</v>
       </c>
-      <c r="J71" s="5">
+      <c r="J72" s="5">
         <f t="shared" si="4"/>
         <v>3.5515811363147451E-2</v>
       </c>

</xml_diff>